<commit_message>
Added new conv net and model saving
</commit_message>
<xml_diff>
--- a/InitialResults.xlsx
+++ b/InitialResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shb20\Desktop\NCEL\EEG_Offline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03EF112-D1DE-4545-ACD8-4887D7311F8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CACDC8-189C-4BC1-8D3B-B49D48A72D6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{55BE3567-2F7F-4323-AF49-60072941776F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{55BE3567-2F7F-4323-AF49-60072941776F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="70">
   <si>
     <t>Bandpass range</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Targets</t>
   </si>
   <si>
-    <t>Classifier</t>
-  </si>
-  <si>
     <t>Wet</t>
   </si>
   <si>
@@ -55,15 +52,9 @@
     <t>All 4</t>
   </si>
   <si>
-    <t>ConvNet</t>
-  </si>
-  <si>
     <t>1.0055, 53.38%</t>
   </si>
   <si>
-    <t>Dry train (loss, accuracy)</t>
-  </si>
-  <si>
     <t>1.6884, 37.44%</t>
   </si>
   <si>
@@ -82,15 +73,6 @@
     <t>Up, Down</t>
   </si>
   <si>
-    <t>Dry test (loss, accuracy)</t>
-  </si>
-  <si>
-    <t>Wet train (loss, accuracy)</t>
-  </si>
-  <si>
-    <t>Wet test (loss, accuracy)</t>
-  </si>
-  <si>
     <t>0.4263, 80.90%</t>
   </si>
   <si>
@@ -112,9 +94,6 @@
     <t>0.8898, 62.24%</t>
   </si>
   <si>
-    <t>SVM</t>
-  </si>
-  <si>
     <t>Up, down</t>
   </si>
   <si>
@@ -161,6 +140,108 @@
   </si>
   <si>
     <t>Data type</t>
+  </si>
+  <si>
+    <t>8-12</t>
+  </si>
+  <si>
+    <t>12-30</t>
+  </si>
+  <si>
+    <t>5-12</t>
+  </si>
+  <si>
+    <t>0.9052, 60.94%</t>
+  </si>
+  <si>
+    <t>1.9375, 29.22%</t>
+  </si>
+  <si>
+    <t>1.2220, 43.50%</t>
+  </si>
+  <si>
+    <t>1.4655, 23.59%</t>
+  </si>
+  <si>
+    <t>0.3507, 86.26%</t>
+  </si>
+  <si>
+    <t>1.5960, 53.57%</t>
+  </si>
+  <si>
+    <t>0.4844, 75.00%</t>
+  </si>
+  <si>
+    <t>0.8665, 52.83%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">72.17%, </t>
+  </si>
+  <si>
+    <t>0.2601, 90.14%</t>
+  </si>
+  <si>
+    <t>2.2754, 43.64%</t>
+  </si>
+  <si>
+    <t>0.5832, 67.27%</t>
+  </si>
+  <si>
+    <t>0.7611, 57.14%</t>
+  </si>
+  <si>
+    <t>Conv Net, dry data (loss, accuracy)</t>
+  </si>
+  <si>
+    <t>Conv Net, wet data (loss, accuracy)</t>
+  </si>
+  <si>
+    <t>SVM, wet data (accuracy)</t>
+  </si>
+  <si>
+    <t>SVM, dry data (accuracy)</t>
+  </si>
+  <si>
+    <t>Train</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>0.4572, 82.82%</t>
+  </si>
+  <si>
+    <t>3.3514, 30.59%</t>
+  </si>
+  <si>
+    <t>1.2419, 44.27%</t>
+  </si>
+  <si>
+    <t>1.3997, 24.62%</t>
+  </si>
+  <si>
+    <t>0.3009, 88.96%</t>
+  </si>
+  <si>
+    <t>1.2578, 59.82%</t>
+  </si>
+  <si>
+    <t>0.6051, 65.80%</t>
+  </si>
+  <si>
+    <t>0.7698, 51.89%</t>
+  </si>
+  <si>
+    <t>0.1512, 93.35%</t>
+  </si>
+  <si>
+    <t>2.6022, 46.36%</t>
+  </si>
+  <si>
+    <t>0.6326, 64.69%</t>
+  </si>
+  <si>
+    <t>0.7136, 44.90%</t>
   </si>
 </sst>
 </file>
@@ -176,7 +257,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,6 +267,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -264,13 +351,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -283,11 +369,39 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -356,15 +470,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>73283</xdr:rowOff>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>60583</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>44450</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>78668</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>501650</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>65968</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -387,7 +501,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6318250" y="257433"/>
+          <a:off x="6165850" y="60583"/>
           <a:ext cx="5740400" cy="2583485"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -444,15 +558,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>457201</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:colOff>349251</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>44895</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>546545</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -475,7 +589,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6375401" y="3441700"/>
+          <a:off x="6267451" y="3117850"/>
           <a:ext cx="5683694" cy="2628900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -531,16 +645,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>412751</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>44451</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>171658</xdr:rowOff>
+      <xdr:colOff>387350</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>31958</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -563,7 +677,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7137401" y="6445251"/>
+          <a:off x="6940551" y="6121401"/>
           <a:ext cx="4851399" cy="2197307"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -619,16 +733,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>323851</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>571501</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>12535</xdr:rowOff>
+      <xdr:colOff>285751</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>158585</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -651,8 +765,360 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7137401" y="8839200"/>
+          <a:off x="6851651" y="8432800"/>
           <a:ext cx="4838700" cy="2222335"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>800101</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>292101</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>134120</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67AFAA6C-E25B-4468-AC77-33AA6A4FECCB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2844801" y="10915650"/>
+          <a:ext cx="3365500" cy="1556520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>247651</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>158751</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>60493</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78C6696E-7616-4456-AF8F-6AF42F41B0FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6775451" y="10712450"/>
+          <a:ext cx="3568700" cy="1686093"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>654051</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>69851</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>598924</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A620C08-A1A8-41A9-8AFD-FE787644B8E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2698751" y="12592051"/>
+          <a:ext cx="3208773" cy="1574799"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>298450</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>332872</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C991232B-6B79-4C8C-B924-F1453D88334B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6216650" y="12496800"/>
+          <a:ext cx="4301622" cy="1968500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>831850</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>72874</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85B7F320-5734-4348-B19A-A18EBD3B058D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2876550" y="14655800"/>
+          <a:ext cx="2616200" cy="1806424"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>761</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B2F75A7-18D7-4F9B-8C02-9109594293F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5918201" y="14732001"/>
+          <a:ext cx="4267960" cy="1943099"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>451897</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{205CA1FF-0DE1-44EF-8529-C92D66F7F126}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2578100" y="16833851"/>
+          <a:ext cx="3182397" cy="1454149"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>521214</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBF65792-BDAA-4E68-8822-36F66181A167}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5918200" y="16941800"/>
+          <a:ext cx="3569214" cy="1651000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -961,10 +1427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9D9B5C9-F632-4D52-8CFE-530F44B328D0}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -978,7 +1444,7 @@
     <col min="7" max="7" width="21.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -986,304 +1452,582 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>18</v>
+        <v>35</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="17">
+        <v>0.49480000000000002</v>
+      </c>
+      <c r="G2" s="18">
+        <v>0.50839999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="8">
-        <v>0.49480000000000002</v>
-      </c>
-      <c r="E3" s="9">
+      <c r="E3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="8">
         <v>0.42470000000000002</v>
       </c>
-      <c r="F3" s="8">
-        <v>0.50839999999999996</v>
-      </c>
-      <c r="G3" s="10">
+      <c r="G3" s="9">
         <v>0.31790000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="17">
+        <v>0.78380000000000005</v>
+      </c>
+      <c r="G4" s="18">
+        <v>0.70750000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="8">
-        <v>0.78380000000000005</v>
-      </c>
-      <c r="E5" s="9">
+      <c r="F5" s="8">
         <v>0.65180000000000005</v>
       </c>
-      <c r="F5" s="8">
-        <v>0.70750000000000002</v>
-      </c>
-      <c r="G5" s="10">
+      <c r="G5" s="9">
         <v>0.55659999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="17">
+        <v>0.69489999999999996</v>
+      </c>
+      <c r="G6" s="18">
+        <v>0.78869999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0.57269999999999999</v>
+      </c>
+      <c r="G7" s="9">
+        <v>0.61219999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="17">
+        <v>0.65749999999999997</v>
+      </c>
+      <c r="G9" s="18">
+        <v>0.51349999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="B10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="12" t="s">
+      <c r="E10" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="11" t="s">
+      <c r="F10" s="8">
+        <v>0.3105</v>
+      </c>
+      <c r="G10" s="9">
+        <v>0.26669999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="17">
+        <v>0.84230000000000005</v>
+      </c>
+      <c r="G11" s="18">
+        <v>0.73580000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0.50890000000000002</v>
+      </c>
+      <c r="G12" s="9">
+        <v>0.41510000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="20">
+        <v>0.8417</v>
+      </c>
+      <c r="G13" s="18">
+        <v>0.7268</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0.47270000000000001</v>
+      </c>
+      <c r="G14" s="9">
+        <v>0.52039999999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="8">
-        <v>0.69489999999999996</v>
-      </c>
-      <c r="E7" s="8">
-        <v>0.57269999999999999</v>
-      </c>
-      <c r="F7" s="8">
-        <v>0.78869999999999996</v>
-      </c>
-      <c r="G7" s="10">
-        <v>0.61219999999999997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="8">
-        <v>0.65749999999999997</v>
-      </c>
-      <c r="E10" s="9">
-        <v>0.3105</v>
-      </c>
-      <c r="F10" s="8">
-        <v>0.51349999999999996</v>
-      </c>
-      <c r="G10" s="10">
-        <v>0.26669999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="8">
-        <v>0.84230000000000005</v>
-      </c>
-      <c r="E12" s="8">
-        <v>0.50890000000000002</v>
-      </c>
-      <c r="F12" s="8">
-        <v>0.73580000000000001</v>
-      </c>
-      <c r="G12" s="10">
-        <v>0.41510000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="3" t="s">
+      <c r="C16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="23">
+        <v>0.51659999999999995</v>
+      </c>
+      <c r="G16" s="18">
+        <v>0.46329999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="E17" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="25">
+        <v>0.25109999999999999</v>
+      </c>
+      <c r="G17" s="15">
+        <v>0.30769999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="17">
+        <v>0.70720000000000005</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="8">
+        <v>0.58040000000000003</v>
+      </c>
+      <c r="G19" s="9">
+        <v>0.3962</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="22">
+        <v>0.75460000000000005</v>
+      </c>
+      <c r="G20" s="18">
+        <v>0.64180000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="7">
+        <v>0.4909</v>
+      </c>
+      <c r="G21" s="15">
+        <v>0.54079999999999995</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="9">
-        <v>0.8417</v>
-      </c>
-      <c r="E14" s="8">
+      <c r="B23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F23" s="23">
+        <v>0.61739999999999995</v>
+      </c>
+      <c r="G23" s="18">
+        <v>0.50449999999999995</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" s="8">
+        <v>0.32419999999999999</v>
+      </c>
+      <c r="G24" s="24">
+        <v>0.18970000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" s="17">
+        <v>0.79279999999999995</v>
+      </c>
+      <c r="G25" s="18">
+        <v>0.69810000000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F26" s="25">
+        <v>0.58930000000000005</v>
+      </c>
+      <c r="G26" s="9">
+        <v>0.3962</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F27" s="23">
+        <v>0.80279999999999996</v>
+      </c>
+      <c r="G27" s="18">
+        <v>0.73970000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F28" s="25">
         <v>0.47270000000000001</v>
       </c>
-      <c r="F14" s="8">
-        <v>0.7268</v>
-      </c>
-      <c r="G14" s="10">
-        <v>0.52039999999999997</v>
+      <c r="G28" s="15">
+        <v>0.54079999999999995</v>
       </c>
     </row>
   </sheetData>
@@ -1293,10 +2037,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{827562EE-520C-4019-8499-5D0ED0BCDC71}">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N96" sqref="N96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1307,42 +2051,77 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B49" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B61" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B70" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" s="1"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B81" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B93" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>